<commit_message>
Moved figures from outer folder to this folder
</commit_message>
<xml_diff>
--- a/examples/DOE/fig3c.xlsx
+++ b/examples/DOE/fig3c.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rubai\Documents\Programming\AI3SD\edbo\examples\DOE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37F99A8-A918-4C70-9303-778CC6BBEF7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466003FF-7BB0-45BD-9005-05DC13690913}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2141,16 +2141,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>87630</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>34290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2477,7 +2477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="AB18" sqref="AB18"/>
     </sheetView>
   </sheetViews>

</xml_diff>